<commit_message>
bubble sheet module completed
</commit_message>
<xml_diff>
--- a/graded_results.xlsx
+++ b/graded_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,300 +436,118 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Question</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Detected Answer</t>
+          <t>Q1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Correct Answer</t>
+          <t>Q2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Is Correct</t>
+          <t>Q3</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Points</t>
+          <t>Q4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Q5</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Q6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Q7</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Q8</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Q9</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Q10</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Q11</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Q12</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Q13</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D2" t="b">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>00301</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
         <v>1</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>No Answer</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D3" t="b">
+      <c r="F2" t="n">
         <v>0</v>
       </c>
-      <c r="E3" t="n">
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="D5" t="b">
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
         <v>0</v>
       </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>No Answer</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>No Answer</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>A,B</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>A,C</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>A,C</t>
-        </is>
-      </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="n">
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>